<commit_message>
Add paper download link
Now v1.0
</commit_message>
<xml_diff>
--- a/AMOSTO.xlsx
+++ b/AMOSTO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SASHA-OPTIPLEX-3010\Professional-shared\NH3 MTC paper\Spreadsheet calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasha\Git-repos\AMOSTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3360DA-0D27-4138-9157-BEDE3BBDD1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A1E8AC-A6B1-4BCF-82C5-221F30D72712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="113">
   <si>
     <t>Livestock type</t>
   </si>
@@ -642,13 +642,16 @@
     <t>https://github.com/sashahafner/AMOSTO</t>
   </si>
   <si>
-    <t>(coming soon)</t>
-  </si>
-  <si>
     <t>Latest version and more information:</t>
   </si>
   <si>
     <t>Change file name, add AMOSTO to Model sheet, hiding this ChangeLog and other sheets except Model and License, add GitHub info to Model sheet</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>Add download link, reformat notes a bit.</t>
   </si>
 </sst>
 </file>
@@ -955,19 +958,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -994,27 +991,27 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1033,7 +1030,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1042,26 +1039,17 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1071,81 +1059,90 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="17" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3329,7 +3326,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P46"/>
+  <dimension ref="B2:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -3337,737 +3334,584 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="29.140625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="9" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="9" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="9"/>
-    <col min="15" max="15" width="21.7109375" style="9" customWidth="1"/>
-    <col min="16" max="1025" width="11.5703125" style="9"/>
-    <col min="1026" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="5.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="29.140625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="7" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="7" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="7"/>
+    <col min="15" max="15" width="21.7109375" style="7" customWidth="1"/>
+    <col min="16" max="1025" width="11.5703125" style="7"/>
+    <col min="1026" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="F4" s="40" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="F4" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="K4" s="43" t="s">
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="K4" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="51"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="11"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="11"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="42" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="9"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="42"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="11"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="F6" s="13" t="s">
+      <c r="D6" s="13"/>
+      <c r="F6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="15">
         <f>INDEX(Parameters!B3:C5,Lookup!C2,Lookup!C3)</f>
         <v>262</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="16" t="s">
+      <c r="H6" s="13"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="L6" s="36">
+      <c r="L6" s="31">
         <f>C7*C10*365.25</f>
         <v>3290.5372500000003</v>
       </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="15"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="13"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="18">
         <v>2.73</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="F7" s="13" t="s">
+      <c r="D7" s="13"/>
+      <c r="F7" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="24">
         <f>VLOOKUP(C16,Parameters!A8:C21,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="16" t="s">
+      <c r="H7" s="13"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="28">
         <f>Calculations!N15</f>
         <v>125.18627820689196</v>
       </c>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="15"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="13"/>
     </row>
     <row r="8" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="15"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="16" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="13"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="34">
+      <c r="L8" s="29">
         <f>100*L7/L6</f>
         <v>3.8044327930611312</v>
       </c>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="15"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="13"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="15"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="15"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="13"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="13"/>
     </row>
     <row r="10" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="12">
         <v>3.3</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="F10" s="40" t="s">
+      <c r="D10" s="13"/>
+      <c r="F10" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="J10" s="46" t="s">
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="J10" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39" t="s">
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="15"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="13"/>
     </row>
     <row r="11" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="18">
         <v>7.2</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="F11" s="47" t="str">
+      <c r="D11" s="13"/>
+      <c r="F11" s="40" t="str">
         <f>Warnings!D4</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="49"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="15"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="42"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="13"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="13"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="15"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="52"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="15"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="13"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="45"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="13"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="15"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="52"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="15"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="13"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="45"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="13"/>
     </row>
     <row r="14" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="15"/>
+      <c r="D14" s="13"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="13"/>
     </row>
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="16">
         <v>333</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="15"/>
+      <c r="D15" s="13"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="45"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="13"/>
     </row>
     <row r="16" spans="2:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="F16" s="53" t="str">
+      <c r="D16" s="13"/>
+      <c r="F16" s="46" t="str">
         <f>IF(LEN(F11)&gt;1,"","No warnings.")</f>
         <v>No warnings.</v>
       </c>
-      <c r="G16" s="54"/>
-      <c r="H16" s="55"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="15"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="48"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="13"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="13"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="15"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="15"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="13"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="13"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="15"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="15"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="13"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="13"/>
     </row>
     <row r="19" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="12">
         <v>0</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="F19" s="40" t="s">
+      <c r="D19" s="13"/>
+      <c r="F19" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="15"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="13"/>
     </row>
     <row r="20" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="16">
         <v>0</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="11"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="15"/>
+      <c r="D20" s="13"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="9"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="13"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="16">
         <v>2.1</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="F21" s="28" t="s">
+      <c r="D21" s="13"/>
+      <c r="F21" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="15"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="15"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="13"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="13"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="16">
         <v>5.7</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="F22" s="62" t="s">
-        <v>110</v>
-      </c>
-      <c r="G22" s="57" t="s">
+      <c r="D22" s="13"/>
+      <c r="F22" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="58"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="15"/>
+      <c r="H22" s="59"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="13"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="16">
         <v>10.8</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="58"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="15"/>
+      <c r="D23" s="13"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="59"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="13"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="16">
         <v>14.3</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="F24" s="28" t="s">
+      <c r="D24" s="13"/>
+      <c r="F24" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="H24" s="15"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="15"/>
+      <c r="G24" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="13"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="16">
         <v>15.6</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="F25" s="28" t="s">
+      <c r="D25" s="13"/>
+      <c r="F25" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="38" t="s">
+      <c r="G25" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="H25" s="15"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="15"/>
+      <c r="H25" s="13"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="13"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="16">
         <v>15.7</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="F26" s="28" t="s">
+      <c r="D26" s="13"/>
+      <c r="F26" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="G26" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="15"/>
+      <c r="H26" s="13"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="13"/>
     </row>
     <row r="27" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="16">
         <v>12.7</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="F27" s="29" t="s">
+      <c r="D27" s="13"/>
+      <c r="F27" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="61">
+      <c r="G27" s="57">
         <f>MAX(ChangeLog!A4:A1011)</f>
-        <v>0.5</v>
-      </c>
-      <c r="H27" s="23"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="H27" s="21"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="21"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="16">
         <v>9.1</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="32"/>
-      <c r="O28" s="32"/>
-      <c r="P28" s="32"/>
+      <c r="D28" s="13"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="16">
         <v>4.7</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="32"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="18">
         <v>1.6</v>
       </c>
-      <c r="D30" s="15"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
+      <c r="D30" s="13"/>
     </row>
     <row r="31" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="23"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="32"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-    </row>
-    <row r="33" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="32"/>
-      <c r="P33" s="32"/>
-    </row>
-    <row r="34" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
-    </row>
-    <row r="35" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="32"/>
-    </row>
-    <row r="36" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-    </row>
-    <row r="37" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
-    </row>
-    <row r="38" spans="10:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-    </row>
-    <row r="39" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
-    </row>
-    <row r="40" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-    </row>
-    <row r="41" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-    </row>
-    <row r="42" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
-      <c r="N42" s="32"/>
-      <c r="O42" s="32"/>
-      <c r="P42" s="32"/>
-    </row>
-    <row r="43" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
-      <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
-    </row>
-    <row r="44" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="32"/>
-      <c r="O44" s="32"/>
-      <c r="P44" s="32"/>
-    </row>
-    <row r="45" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
-      <c r="O45" s="32"/>
-      <c r="P45" s="32"/>
-    </row>
-    <row r="46" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="32"/>
-      <c r="O46" s="32"/>
-      <c r="P46" s="32"/>
-    </row>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="38" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="18">
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B9:C9"/>
@@ -4079,24 +3923,18 @@
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="G22:H23"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G22" r:id="rId1" xr:uid="{34DB199A-A3BF-4DC7-A0C6-1DB159FEB52F}"/>
+    <hyperlink ref="G24" r:id="rId2" display="(link)" xr:uid="{1CF429E3-5056-44D7-8445-E982C065AE94}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -4136,7 +3974,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="293.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="30" t="s">
         <v>100</v>
       </c>
     </row>
@@ -4163,10 +4001,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="56"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -4213,10 +4051,10 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="56"/>
+      <c r="C7" s="52"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -4398,7 +4236,7 @@
         <f>Model!C6</f>
         <v>Pig</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <f>MATCH(B2,Parameters!A3:A5)</f>
         <v>2</v>
       </c>
@@ -4411,7 +4249,7 @@
         <f>Model!C14</f>
         <v>Tank</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <f>MATCH(B3,Parameters!B2:C2)</f>
         <v>2</v>
       </c>
@@ -4431,760 +4269,760 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="2" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="1030" width="11.5703125" style="2"/>
-    <col min="1031" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="1030" width="11.5703125" style="1"/>
+    <col min="1031" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>31</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <f>Model!C19</f>
         <v>0</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5">
         <f>EXP((14.01708-(10294.83/(C3+273.15))-0.039282*(C3+273.15))-(191.97-8451/(C3+273.15)-31.4335*LN(C3+273.15)+0.0152123*(C3+273.15)))</f>
         <v>8.0265030359107485E-11</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="5">
         <f>EXP(-(160.559-(8621.06/(273.15+C3))-(25.6767*LN(273.15+C3))+(0.035388*(273.15+C3))))</f>
         <v>217.72422704130878</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="5">
         <f t="shared" ref="K3:K14" si="0">J3*0.08205746*(273.15+C3)</f>
         <v>4880.0697796098802</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="5">
         <f>($D3/(1+(10^-E3)/$I3))*1/$K3</f>
         <v>8.5913648131857518E-7</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="5">
         <f>1000*L3/F3*G3*86400</f>
         <v>0.28331829002261411</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="5">
         <f>M3*B3*H3/1000</f>
         <v>2.9246947079034458</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>28.25</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <f>Model!C20</f>
         <v>0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <f t="shared" ref="I4:I14" si="1">EXP((14.01708-(10294.83/(C4+273.15))-0.039282*(C4+273.15))-(191.97-8451/(C4+273.15)-31.4335*LN(C4+273.15)+0.0152123*(C4+273.15)))</f>
         <v>8.0265030359107485E-11</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="5">
         <f t="shared" ref="J4:J14" si="2">EXP(-(160.559-(8621.06/(273.15+C4))-(25.6767*LN(273.15+C4))+(0.035388*(273.15+C4))))</f>
         <v>217.72422704130878</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="5">
         <f t="shared" si="0"/>
         <v>4880.0697796098802</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="5">
         <f t="shared" ref="L4:L14" si="3">($D4/(1+(10^-E4)/$I4))*1/$K4</f>
         <v>8.5913648131857518E-7</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="5">
         <f t="shared" ref="M4:M14" si="4">1000*L4/F4*G4*86400</f>
         <v>0.28331829002261411</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="5">
         <f t="shared" ref="N4:N14" si="5">M4*B4*H4/1000</f>
         <v>2.6652459838152369</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>31</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <f>Model!C21</f>
         <v>2.1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <f t="shared" si="1"/>
         <v>9.5883668800187196E-11</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="5">
         <f t="shared" si="2"/>
         <v>193.4012213630125</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="5">
         <f t="shared" si="0"/>
         <v>4368.2210743817859</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="5">
         <f t="shared" si="3"/>
         <v>1.1462899820864319E-6</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="5">
         <f t="shared" si="4"/>
         <v>0.37801318493231956</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="5">
         <f t="shared" si="5"/>
         <v>3.9022301080563349</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>30</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <f>Model!C22</f>
         <v>5.7</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="5">
         <f t="shared" si="1"/>
         <v>1.2926856903372692E-10</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="5">
         <f t="shared" si="2"/>
         <v>158.64385147659752</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="5">
         <f t="shared" si="0"/>
         <v>3630.0446208790099</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="5">
         <f t="shared" si="3"/>
         <v>1.8586861336892291E-6</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="5">
         <f t="shared" si="4"/>
         <v>0.61294077080438703</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="5">
         <f t="shared" si="5"/>
         <v>6.1232783003358264</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>31</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <f>Model!C23</f>
         <v>10.8</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="5">
         <f t="shared" si="1"/>
         <v>1.9489080256713852E-10</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="5">
         <f t="shared" si="2"/>
         <v>121.05725647099281</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="5">
         <f t="shared" si="0"/>
         <v>2820.6601959351892</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="5">
         <f t="shared" si="3"/>
         <v>3.6025923944984685E-6</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="5">
         <f t="shared" si="4"/>
         <v>1.1880304690254493</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="5">
         <f t="shared" si="5"/>
         <v>12.264038531749714</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>30</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <f>Model!C24</f>
         <v>14.3</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="5">
         <f t="shared" si="1"/>
         <v>2.5617451045023703E-10</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="5">
         <f t="shared" si="2"/>
         <v>101.21895900896651</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="5">
         <f t="shared" si="0"/>
         <v>2387.4937820004675</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="5">
         <f t="shared" si="3"/>
         <v>5.5891774707089577E-6</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="5">
         <f t="shared" si="4"/>
         <v>1.8431486010276867</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="5">
         <f t="shared" si="5"/>
         <v>18.413054524266592</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>31</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <f>Model!C25</f>
         <v>15.6</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="5">
         <f t="shared" si="1"/>
         <v>2.8308111253051739E-10</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="5">
         <f t="shared" si="2"/>
         <v>94.832928905220058</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="5">
         <f t="shared" si="0"/>
         <v>2246.9801018057487</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="5">
         <f t="shared" si="3"/>
         <v>6.5596623977040859E-6</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="5">
         <f t="shared" si="4"/>
         <v>2.1631863784795153</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="5">
         <f t="shared" si="5"/>
         <v>22.330572985044039</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>31</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <f>Model!C26</f>
         <v>15.7</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="5">
         <f t="shared" si="1"/>
         <v>2.8525368367534082E-10</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="5">
         <f t="shared" si="2"/>
         <v>94.361428755838304</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="5">
         <f t="shared" si="0"/>
         <v>2236.5826400052383</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="5">
         <f t="shared" si="3"/>
         <v>6.6405071092304341E-6</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="5">
         <f t="shared" si="4"/>
         <v>2.1898466192271355</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="5">
         <f t="shared" si="5"/>
         <v>22.605786650281718</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>30</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <f>Model!C27</f>
         <v>12.7</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="5">
         <f t="shared" si="1"/>
         <v>2.2626175389821364E-10</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="5">
         <f t="shared" si="2"/>
         <v>109.77788398665122</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="5">
         <f t="shared" si="0"/>
         <v>2574.9637625494938</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="5">
         <f t="shared" si="3"/>
         <v>4.5793028907589869E-6</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="5">
         <f t="shared" si="4"/>
         <v>1.5101212586319712</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="5">
         <f t="shared" si="5"/>
         <v>15.086111373733392</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>31</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <f>Model!C28</f>
         <v>9.1</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="5">
         <f t="shared" si="1"/>
         <v>1.7024050227914191E-10</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="5">
         <f t="shared" si="2"/>
         <v>132.30394953776198</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="5">
         <f t="shared" si="0"/>
         <v>3064.2544767761715</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="5">
         <f t="shared" si="3"/>
         <v>2.8978893414938787E-6</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="5">
         <f t="shared" si="4"/>
         <v>0.95563984391248524</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="5">
         <f t="shared" si="5"/>
         <v>9.8650701087085846</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>30</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <f>Model!C29</f>
         <v>4.7</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="5">
         <f t="shared" si="1"/>
         <v>1.1906391091978929E-10</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="5">
         <f t="shared" si="2"/>
         <v>167.51517792853946</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="5">
         <f t="shared" si="0"/>
         <v>3819.2899829075541</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="5">
         <f t="shared" si="3"/>
         <v>1.6273939342049706E-6</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="5">
         <f t="shared" si="4"/>
         <v>0.53666731265385292</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="5">
         <f t="shared" si="5"/>
         <v>5.3613064534119914</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>31</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <f>Model!C30</f>
         <v>1.6</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <f>Model!C$10</f>
         <v>3.3</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="4">
         <f>Model!C$11</f>
         <v>7.2</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="4">
         <f>Model!G$6</f>
         <v>262</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="4">
         <f>Model!G$7</f>
         <v>1</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="4">
         <f>Model!C$15</f>
         <v>333</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="5">
         <f t="shared" si="1"/>
         <v>9.1931190490768314E-11</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="5">
         <f t="shared" si="2"/>
         <v>198.89454649789792</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="5">
         <f t="shared" si="0"/>
         <v>4484.1346603807169</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="5">
         <f t="shared" si="3"/>
         <v>1.070695226646106E-6</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="5">
         <f t="shared" si="4"/>
         <v>0.353084227413067</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="5">
         <f t="shared" si="5"/>
         <v>3.6448884795850902</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <f>SUM(B3:B14)</f>
         <v>365.25</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="8">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="6">
         <f>SUM(N3:N14)</f>
         <v>125.18627820689196</v>
       </c>
@@ -5209,101 +5047,101 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="12.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="4"/>
-    <col min="9" max="9" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <f>IF(LEN(C2)&gt;1,1,0)</f>
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="str">
+      <c r="C2" s="5" t="str">
         <f>IF(I2&gt;H2,CONCATENATE("Check inputs. Values imply a long storage period of &gt; ",ROUND(I2,0)," days."),"")</f>
         <v/>
       </c>
-      <c r="D2" s="7" t="str">
+      <c r="D2" s="5" t="str">
         <f>IF(LEN(C2)&gt;1,CONCATENATE(B2,". ",C2),"")</f>
         <v/>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="1">
         <v>365</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="5">
         <f>Model!C15*Warnings!G2/Model!C7</f>
         <v>121.97802197802199</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <f>IF(LEN(C3)&gt;1,B2+1,B2)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="str">
+      <c r="C3" s="5" t="str">
         <f>IF(Model!L8&gt;Warnings!G5,CONCATENATE("Model assumes constant emission rate and is less accurate for high losses. Calculated loss is ",ROUND(Model!L8,0),"% of TAN flow."),"")</f>
         <v/>
       </c>
-      <c r="D3" s="7" t="str">
+      <c r="D3" s="5" t="str">
         <f>IF(LEN(C3)&gt;1,CONCATENATE(B3,". ",C3),"")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37" t="str">
+      <c r="B4" s="5"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32" t="str">
         <f>CONCATENATE(D2, " ", D3)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G5" s="4">
+      <c r="G5" s="1">
         <v>20</v>
       </c>
     </row>
@@ -5315,10 +5153,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252B4D1B-B8A9-457A-97D9-39EFD218058D}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5349,7 +5187,7 @@
       <c r="A2">
         <v>0.1</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="27">
         <v>44583</v>
       </c>
       <c r="C2" t="s">
@@ -5366,7 +5204,7 @@
       <c r="A3">
         <v>0.2</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="27">
         <v>44586</v>
       </c>
       <c r="C3" t="s">
@@ -5383,7 +5221,7 @@
       <c r="A4">
         <v>0.3</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="27">
         <v>44586</v>
       </c>
       <c r="C4" t="s">
@@ -5400,7 +5238,7 @@
       <c r="A5">
         <v>0.3</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="27">
         <v>44586</v>
       </c>
       <c r="C5" t="s">
@@ -5417,7 +5255,7 @@
       <c r="A6">
         <v>0.4</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="27">
         <v>44587</v>
       </c>
       <c r="C6" t="s">
@@ -5434,7 +5272,7 @@
       <c r="A7">
         <v>0.5</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="27">
         <v>44799</v>
       </c>
       <c r="C7" t="s">
@@ -5444,7 +5282,24 @@
         <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="27">
+        <v>44819</v>
+      </c>
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.1 fix lookup behavior based on feedback from M. Berglund
</commit_message>
<xml_diff>
--- a/AMOSTO.xlsx
+++ b/AMOSTO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasha\Git-repos\AMOSTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A1E8AC-A6B1-4BCF-82C5-221F30D72712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D6DC62-4DFC-40CF-B930-78CFBF6D2EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="114">
   <si>
     <t>Livestock type</t>
   </si>
@@ -652,6 +652,9 @@
   </si>
   <si>
     <t>Add download link, reformat notes a bit.</t>
+  </si>
+  <si>
+    <t>Fix lookup behavior in "Lookup" for cattle/digestate based on user feedback</t>
   </si>
 </sst>
 </file>
@@ -1059,63 +1062,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -1132,6 +1078,60 @@
     <xf numFmtId="164" fontId="17" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1143,6 +1143,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1211,40 +1214,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.9246947079034458</c:v>
+                  <c:v>5.8493894158068915</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6652459838152369</c:v>
+                  <c:v>5.3304919676304738</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9022301080563349</c:v>
+                  <c:v>7.8044602161126697</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.1232783003358264</c:v>
+                  <c:v>12.246556600671653</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.264038531749714</c:v>
+                  <c:v>24.528077063499428</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.413054524266592</c:v>
+                  <c:v>36.826109048533183</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.330572985044039</c:v>
+                  <c:v>44.661145970088079</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.605786650281718</c:v>
+                  <c:v>45.211573300563437</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.086111373733392</c:v>
+                  <c:v>30.172222747466783</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.8650701087085846</c:v>
+                  <c:v>19.730140217417169</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.3613064534119914</c:v>
+                  <c:v>10.722612906823983</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.6448884795850902</c:v>
+                  <c:v>7.2897769591701804</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1586,40 +1589,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.28331829002261411</c:v>
+                  <c:v>0.56663658004522821</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28331829002261411</c:v>
+                  <c:v>0.56663658004522821</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37801318493231956</c:v>
+                  <c:v>0.75602636986463911</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.61294077080438703</c:v>
+                  <c:v>1.2258815416087741</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1880304690254493</c:v>
+                  <c:v>2.3760609380508986</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8431486010276867</c:v>
+                  <c:v>3.6862972020553735</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1631863784795153</c:v>
+                  <c:v>4.3263727569590307</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1898466192271355</c:v>
+                  <c:v>4.3796932384542711</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5101212586319712</c:v>
+                  <c:v>3.0202425172639424</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.95563984391248524</c:v>
+                  <c:v>1.9112796878249705</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.53666731265385292</c:v>
+                  <c:v>1.0733346253077058</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.353084227413067</c:v>
+                  <c:v>0.706168454826134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3354,18 +3357,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B3" s="8"/>
@@ -3380,35 +3383,35 @@
       <c r="K3" s="8"/>
     </row>
     <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="F4" s="39" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="F4" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="K4" s="51" t="s">
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="K4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="51"/>
+      <c r="L4" s="43"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="9"/>
       <c r="F5" s="22"/>
       <c r="G5" s="23"/>
       <c r="H5" s="9"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="36"/>
+      <c r="L5" s="42"/>
       <c r="M5" s="25"/>
       <c r="N5" s="25"/>
       <c r="O5" s="25"/>
@@ -3419,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="13"/>
       <c r="F6" s="11" t="s">
@@ -3427,7 +3430,7 @@
       </c>
       <c r="G6" s="15">
         <f>INDEX(Parameters!B3:C5,Lookup!C2,Lookup!C3)</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="H6" s="13"/>
       <c r="J6" s="11"/>
@@ -3465,7 +3468,7 @@
       </c>
       <c r="L7" s="28">
         <f>Calculations!N15</f>
-        <v>125.18627820689196</v>
+        <v>250.37255641378391</v>
       </c>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
@@ -3485,7 +3488,7 @@
       </c>
       <c r="L8" s="29">
         <f>100*L7/L6</f>
-        <v>3.8044327930611312</v>
+        <v>7.6088655861222625</v>
       </c>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
@@ -3493,10 +3496,10 @@
       <c r="P8" s="13"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="38"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="13"/>
       <c r="J9" s="11"/>
       <c r="K9" s="14"/>
@@ -3514,21 +3517,21 @@
         <v>3.3</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="J10" s="37" t="s">
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="J10" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38" t="s">
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
       <c r="P10" s="13"/>
     </row>
     <row r="11" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3539,12 +3542,12 @@
         <v>7.2</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="F11" s="40" t="str">
+      <c r="F11" s="47" t="str">
         <f>Warnings!D4</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="49"/>
       <c r="J11" s="11"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
@@ -3557,9 +3560,9 @@
       <c r="B12" s="11"/>
       <c r="C12" s="14"/>
       <c r="D12" s="13"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="45"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
       <c r="J12" s="11"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
@@ -3569,14 +3572,14 @@
       <c r="P12" s="13"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="13"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="45"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="52"/>
       <c r="J13" s="11"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
@@ -3593,9 +3596,9 @@
         <v>6</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="45"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="52"/>
       <c r="J14" s="11"/>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
@@ -3612,9 +3615,9 @@
         <v>333</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="45"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="52"/>
       <c r="J15" s="11"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -3631,12 +3634,12 @@
         <v>25</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="F16" s="46" t="str">
+      <c r="F16" s="53" t="str">
         <f>IF(LEN(F11)&gt;1,"","No warnings.")</f>
         <v>No warnings.</v>
       </c>
-      <c r="G16" s="47"/>
-      <c r="H16" s="48"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="55"/>
       <c r="J16" s="11"/>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -3658,10 +3661,10 @@
       <c r="P17" s="13"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="38"/>
+      <c r="C18" s="39"/>
       <c r="D18" s="13"/>
       <c r="J18" s="11"/>
       <c r="K18" s="14"/>
@@ -3679,11 +3682,11 @@
         <v>0</v>
       </c>
       <c r="D19" s="13"/>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
       <c r="J19" s="11"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
@@ -3740,13 +3743,13 @@
         <v>5.7</v>
       </c>
       <c r="D22" s="13"/>
-      <c r="F22" s="49" t="s">
+      <c r="F22" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="G22" s="58" t="s">
+      <c r="G22" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="59"/>
+      <c r="H22" s="58"/>
       <c r="J22" s="11"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
@@ -3763,9 +3766,9 @@
         <v>10.8</v>
       </c>
       <c r="D23" s="13"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="59"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="58"/>
       <c r="J23" s="11"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -3782,10 +3785,10 @@
         <v>14.3</v>
       </c>
       <c r="D24" s="13"/>
-      <c r="F24" s="54" t="s">
+      <c r="F24" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="53" t="s">
+      <c r="G24" s="34" t="s">
         <v>111</v>
       </c>
       <c r="H24" s="13"/>
@@ -3805,7 +3808,7 @@
         <v>15.6</v>
       </c>
       <c r="D25" s="13"/>
-      <c r="F25" s="54" t="s">
+      <c r="F25" s="35" t="s">
         <v>83</v>
       </c>
       <c r="G25" s="33" t="s">
@@ -3828,10 +3831,10 @@
         <v>15.7</v>
       </c>
       <c r="D26" s="13"/>
-      <c r="F26" s="54" t="s">
+      <c r="F26" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="G26" s="56" t="s">
+      <c r="G26" s="37" t="s">
         <v>99</v>
       </c>
       <c r="H26" s="13"/>
@@ -3851,12 +3854,12 @@
         <v>12.7</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="F27" s="55" t="s">
+      <c r="F27" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="57">
+      <c r="G27" s="38">
         <f>MAX(ChangeLog!A4:A1011)</f>
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H27" s="21"/>
       <c r="J27" s="19"/>
@@ -3875,8 +3878,8 @@
         <v>9.1</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="11" t="s">
@@ -3905,13 +3908,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F4:H4"/>
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B9:C9"/>
@@ -3923,6 +3919,13 @@
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="G22:H23"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G22" r:id="rId1" xr:uid="{34DB199A-A3BF-4DC7-A0C6-1DB159FEB52F}"/>
@@ -3988,7 +3991,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4001,10 +4004,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="52"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -4051,10 +4054,10 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="52"/>
+      <c r="C7" s="60"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -4215,7 +4218,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4234,11 +4237,11 @@
       </c>
       <c r="B2" t="str">
         <f>Model!C6</f>
-        <v>Pig</v>
+        <v>Cattle</v>
       </c>
       <c r="C2" s="2">
-        <f>MATCH(B2,Parameters!A3:A5)</f>
-        <v>2</v>
+        <f>MATCH(B2,Parameters!A3:A5,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -4250,7 +4253,7 @@
         <v>Tank</v>
       </c>
       <c r="C3" s="2">
-        <f>MATCH(B3,Parameters!B2:C2)</f>
+        <f>MATCH(B3,Parameters!B2:C2,0)</f>
         <v>2</v>
       </c>
     </row>
@@ -4352,7 +4355,7 @@
       </c>
       <c r="F3" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G3" s="4">
         <f>Model!G$7</f>
@@ -4380,11 +4383,11 @@
       </c>
       <c r="M3" s="5">
         <f>1000*L3/F3*G3*86400</f>
-        <v>0.28331829002261411</v>
+        <v>0.56663658004522821</v>
       </c>
       <c r="N3" s="5">
         <f>M3*B3*H3/1000</f>
-        <v>2.9246947079034458</v>
+        <v>5.8493894158068915</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -4408,7 +4411,7 @@
       </c>
       <c r="F4" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G4" s="4">
         <f>Model!G$7</f>
@@ -4436,11 +4439,11 @@
       </c>
       <c r="M4" s="5">
         <f t="shared" ref="M4:M14" si="4">1000*L4/F4*G4*86400</f>
-        <v>0.28331829002261411</v>
+        <v>0.56663658004522821</v>
       </c>
       <c r="N4" s="5">
         <f t="shared" ref="N4:N14" si="5">M4*B4*H4/1000</f>
-        <v>2.6652459838152369</v>
+        <v>5.3304919676304738</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -4464,7 +4467,7 @@
       </c>
       <c r="F5" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G5" s="4">
         <f>Model!G$7</f>
@@ -4492,11 +4495,11 @@
       </c>
       <c r="M5" s="5">
         <f t="shared" si="4"/>
-        <v>0.37801318493231956</v>
+        <v>0.75602636986463911</v>
       </c>
       <c r="N5" s="5">
         <f t="shared" si="5"/>
-        <v>3.9022301080563349</v>
+        <v>7.8044602161126697</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -4520,7 +4523,7 @@
       </c>
       <c r="F6" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G6" s="4">
         <f>Model!G$7</f>
@@ -4548,11 +4551,11 @@
       </c>
       <c r="M6" s="5">
         <f t="shared" si="4"/>
-        <v>0.61294077080438703</v>
+        <v>1.2258815416087741</v>
       </c>
       <c r="N6" s="5">
         <f t="shared" si="5"/>
-        <v>6.1232783003358264</v>
+        <v>12.246556600671653</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -4576,7 +4579,7 @@
       </c>
       <c r="F7" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G7" s="4">
         <f>Model!G$7</f>
@@ -4604,11 +4607,11 @@
       </c>
       <c r="M7" s="5">
         <f t="shared" si="4"/>
-        <v>1.1880304690254493</v>
+        <v>2.3760609380508986</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="5"/>
-        <v>12.264038531749714</v>
+        <v>24.528077063499428</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -4632,7 +4635,7 @@
       </c>
       <c r="F8" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G8" s="4">
         <f>Model!G$7</f>
@@ -4660,11 +4663,11 @@
       </c>
       <c r="M8" s="5">
         <f t="shared" si="4"/>
-        <v>1.8431486010276867</v>
+        <v>3.6862972020553735</v>
       </c>
       <c r="N8" s="5">
         <f t="shared" si="5"/>
-        <v>18.413054524266592</v>
+        <v>36.826109048533183</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -4688,7 +4691,7 @@
       </c>
       <c r="F9" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G9" s="4">
         <f>Model!G$7</f>
@@ -4716,11 +4719,11 @@
       </c>
       <c r="M9" s="5">
         <f t="shared" si="4"/>
-        <v>2.1631863784795153</v>
+        <v>4.3263727569590307</v>
       </c>
       <c r="N9" s="5">
         <f t="shared" si="5"/>
-        <v>22.330572985044039</v>
+        <v>44.661145970088079</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -4744,7 +4747,7 @@
       </c>
       <c r="F10" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G10" s="4">
         <f>Model!G$7</f>
@@ -4772,11 +4775,11 @@
       </c>
       <c r="M10" s="5">
         <f t="shared" si="4"/>
-        <v>2.1898466192271355</v>
+        <v>4.3796932384542711</v>
       </c>
       <c r="N10" s="5">
         <f t="shared" si="5"/>
-        <v>22.605786650281718</v>
+        <v>45.211573300563437</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -4800,7 +4803,7 @@
       </c>
       <c r="F11" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G11" s="4">
         <f>Model!G$7</f>
@@ -4828,11 +4831,11 @@
       </c>
       <c r="M11" s="5">
         <f t="shared" si="4"/>
-        <v>1.5101212586319712</v>
+        <v>3.0202425172639424</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="5"/>
-        <v>15.086111373733392</v>
+        <v>30.172222747466783</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -4856,7 +4859,7 @@
       </c>
       <c r="F12" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G12" s="4">
         <f>Model!G$7</f>
@@ -4884,11 +4887,11 @@
       </c>
       <c r="M12" s="5">
         <f t="shared" si="4"/>
-        <v>0.95563984391248524</v>
+        <v>1.9112796878249705</v>
       </c>
       <c r="N12" s="5">
         <f t="shared" si="5"/>
-        <v>9.8650701087085846</v>
+        <v>19.730140217417169</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -4912,7 +4915,7 @@
       </c>
       <c r="F13" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G13" s="4">
         <f>Model!G$7</f>
@@ -4940,11 +4943,11 @@
       </c>
       <c r="M13" s="5">
         <f t="shared" si="4"/>
-        <v>0.53666731265385292</v>
+        <v>1.0733346253077058</v>
       </c>
       <c r="N13" s="5">
         <f t="shared" si="5"/>
-        <v>5.3613064534119914</v>
+        <v>10.722612906823983</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -4968,7 +4971,7 @@
       </c>
       <c r="F14" s="4">
         <f>Model!G$6</f>
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="G14" s="4">
         <f>Model!G$7</f>
@@ -4996,11 +4999,11 @@
       </c>
       <c r="M14" s="5">
         <f t="shared" si="4"/>
-        <v>0.353084227413067</v>
+        <v>0.706168454826134</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="5"/>
-        <v>3.6448884795850902</v>
+        <v>7.2897769591701804</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -5024,7 +5027,7 @@
       <c r="M15" s="5"/>
       <c r="N15" s="6">
         <f>SUM(N3:N14)</f>
-        <v>125.18627820689196</v>
+        <v>250.37255641378391</v>
       </c>
     </row>
   </sheetData>
@@ -5153,10 +5156,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252B4D1B-B8A9-457A-97D9-39EFD218058D}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5302,6 +5305,23 @@
         <v>112</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B9" s="27">
+        <v>45033</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
v1.2 switch to XMATCH
</commit_message>
<xml_diff>
--- a/AMOSTO.xlsx
+++ b/AMOSTO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasha\Git-repos\AMOSTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D6DC62-4DFC-40CF-B930-78CFBF6D2EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D50155F-78CD-44BD-B885-ABF47B35FE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
   <si>
     <t>Livestock type</t>
   </si>
@@ -654,7 +654,10 @@
     <t>Add download link, reformat notes a bit.</t>
   </si>
   <si>
-    <t>Fix lookup behavior in "Lookup" for cattle/digestate based on user feedback</t>
+    <t>Fix lookup behavior in "MATCH()" for cattle/digestate based on user feedback (end with ,0)</t>
+  </si>
+  <si>
+    <t>Switch MATCH() to XMATCH() based on MS Excel help file</t>
   </si>
 </sst>
 </file>
@@ -1078,28 +1081,22 @@
     <xf numFmtId="164" fontId="17" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1143,6 +1140,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3357,18 +3360,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B3" s="8"/>
@@ -3383,35 +3386,35 @@
       <c r="K3" s="8"/>
     </row>
     <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="F4" s="40" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="F4" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="K4" s="43" t="s">
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="K4" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="59"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="42"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="9"/>
       <c r="F5" s="22"/>
       <c r="G5" s="23"/>
       <c r="H5" s="9"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="42"/>
+      <c r="L5" s="41"/>
       <c r="M5" s="25"/>
       <c r="N5" s="25"/>
       <c r="O5" s="25"/>
@@ -3496,10 +3499,10 @@
       <c r="P8" s="13"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="39"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="13"/>
       <c r="J9" s="11"/>
       <c r="K9" s="14"/>
@@ -3517,21 +3520,21 @@
         <v>3.3</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="J10" s="46" t="s">
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="J10" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39" t="s">
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
       <c r="P10" s="13"/>
     </row>
     <row r="11" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3542,12 +3545,12 @@
         <v>7.2</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="F11" s="47" t="str">
+      <c r="F11" s="45" t="str">
         <f>Warnings!D4</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="49"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="47"/>
       <c r="J11" s="11"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
@@ -3560,9 +3563,9 @@
       <c r="B12" s="11"/>
       <c r="C12" s="14"/>
       <c r="D12" s="13"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="52"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="50"/>
       <c r="J12" s="11"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
@@ -3572,14 +3575,14 @@
       <c r="P12" s="13"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="39"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="13"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="52"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="50"/>
       <c r="J13" s="11"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
@@ -3596,9 +3599,9 @@
         <v>6</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="50"/>
       <c r="J14" s="11"/>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
@@ -3615,9 +3618,9 @@
         <v>333</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="50"/>
       <c r="J15" s="11"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -3634,12 +3637,12 @@
         <v>25</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="F16" s="53" t="str">
+      <c r="F16" s="51" t="str">
         <f>IF(LEN(F11)&gt;1,"","No warnings.")</f>
         <v>No warnings.</v>
       </c>
-      <c r="G16" s="54"/>
-      <c r="H16" s="55"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="53"/>
       <c r="J16" s="11"/>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -3661,10 +3664,10 @@
       <c r="P17" s="13"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="39"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="13"/>
       <c r="J18" s="11"/>
       <c r="K18" s="14"/>
@@ -3682,11 +3685,11 @@
         <v>0</v>
       </c>
       <c r="D19" s="13"/>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
       <c r="J19" s="11"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
@@ -3743,13 +3746,13 @@
         <v>5.7</v>
       </c>
       <c r="D22" s="13"/>
-      <c r="F22" s="56" t="s">
+      <c r="F22" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="G22" s="57" t="s">
+      <c r="G22" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="58"/>
+      <c r="H22" s="56"/>
       <c r="J22" s="11"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
@@ -3766,9 +3769,9 @@
         <v>10.8</v>
       </c>
       <c r="D23" s="13"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="58"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="56"/>
       <c r="J23" s="11"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -3859,7 +3862,7 @@
       </c>
       <c r="G27" s="38">
         <f>MAX(ChangeLog!A4:A1011)</f>
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="H27" s="21"/>
       <c r="J27" s="19"/>
@@ -3878,8 +3881,8 @@
         <v>9.1</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="11" t="s">
@@ -3908,6 +3911,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="18">
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B9:C9"/>
@@ -3919,13 +3929,6 @@
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="G22:H23"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G22" r:id="rId1" xr:uid="{34DB199A-A3BF-4DC7-A0C6-1DB159FEB52F}"/>
@@ -4218,7 +4221,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4240,7 +4243,7 @@
         <v>Cattle</v>
       </c>
       <c r="C2" s="2">
-        <f>MATCH(B2,Parameters!A3:A5,0)</f>
+        <f>_xlfn.XMATCH(B2,Parameters!A3:A5)</f>
         <v>1</v>
       </c>
     </row>
@@ -4253,7 +4256,7 @@
         <v>Tank</v>
       </c>
       <c r="C3" s="2">
-        <f>MATCH(B3,Parameters!B2:C2,0)</f>
+        <f>_xlfn.XMATCH(B3,Parameters!B2:C2)</f>
         <v>2</v>
       </c>
     </row>
@@ -5156,10 +5159,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252B4D1B-B8A9-457A-97D9-39EFD218058D}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5322,6 +5325,23 @@
         <v>113</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1.2</v>
+      </c>
+      <c r="B10" s="27">
+        <v>45033</v>
+      </c>
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
use MATCH(...,0) instead of XMATCH().
See issue #3
</commit_message>
<xml_diff>
--- a/AMOSTO.xlsx
+++ b/AMOSTO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasha\Git-repos\AMOSTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D50155F-78CD-44BD-B885-ABF47B35FE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144EF5DD-66B6-4343-B3A0-005B5A000222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="116">
   <si>
     <t>Livestock type</t>
   </si>
@@ -658,6 +658,9 @@
   </si>
   <si>
     <t>Switch MATCH() to XMATCH() based on MS Excel help file</t>
+  </si>
+  <si>
+    <t>Switch back to MATCH(…,0). See issue #3.</t>
   </si>
 </sst>
 </file>
@@ -1081,22 +1084,28 @@
     <xf numFmtId="164" fontId="17" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,12 +1149,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1217,40 +1220,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>5.8493894158068915</c:v>
+                  <c:v>6.4938136734805321</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3304919676304738</c:v>
+                  <c:v>5.9177495572846777</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.8044602161126697</c:v>
+                  <c:v>8.6642736297522003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.246556600671653</c:v>
+                  <c:v>13.59575351430497</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.528077063499428</c:v>
+                  <c:v>27.230322841681563</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.826109048533183</c:v>
+                  <c:v>40.883222757269891</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44.661145970088079</c:v>
+                  <c:v>49.581441712555403</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45.211573300563437</c:v>
+                  <c:v>50.192509342150935</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30.172222747466783</c:v>
+                  <c:v>33.496281185747023</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.730140217417169</c:v>
+                  <c:v>21.90379973289533</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.722612906823983</c:v>
+                  <c:v>11.903917718592725</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.2897769591701804</c:v>
+                  <c:v>8.0928879800957088</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1592,40 +1595,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.56663658004522821</c:v>
+                  <c:v>0.62906264394851608</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56663658004522821</c:v>
+                  <c:v>0.62906264394851608</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75602636986463911</c:v>
+                  <c:v>0.83931741061243825</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2258815416087741</c:v>
+                  <c:v>1.3609362877182152</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3760609380508986</c:v>
+                  <c:v>2.6378303634293871</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6862972020553735</c:v>
+                  <c:v>4.0924146904174066</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.3263727569590307</c:v>
+                  <c:v>4.8030070437426522</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.3796932384542711</c:v>
+                  <c:v>4.8622018155721145</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0202425172639424</c:v>
+                  <c:v>3.3529810996743765</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9112796878249705</c:v>
+                  <c:v>2.1218443991955178</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0733346253077058</c:v>
+                  <c:v>1.191583355214487</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.706168454826134</c:v>
+                  <c:v>0.78396667442562329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3360,18 +3363,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B3" s="8"/>
@@ -3386,35 +3389,35 @@
       <c r="K3" s="8"/>
     </row>
     <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="F4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="F4" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="K4" s="59" t="s">
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="K4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="59"/>
+      <c r="L4" s="43"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="9"/>
       <c r="F5" s="22"/>
       <c r="G5" s="23"/>
       <c r="H5" s="9"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="41"/>
+      <c r="L5" s="42"/>
       <c r="M5" s="25"/>
       <c r="N5" s="25"/>
       <c r="O5" s="25"/>
@@ -3433,7 +3436,7 @@
       </c>
       <c r="G6" s="15">
         <f>INDEX(Parameters!B3:C5,Lookup!C2,Lookup!C3)</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="H6" s="13"/>
       <c r="J6" s="11"/>
@@ -3471,7 +3474,7 @@
       </c>
       <c r="L7" s="28">
         <f>Calculations!N15</f>
-        <v>250.37255641378391</v>
+        <v>277.95597364581096</v>
       </c>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
@@ -3491,7 +3494,7 @@
       </c>
       <c r="L8" s="29">
         <f>100*L7/L6</f>
-        <v>7.6088655861222625</v>
+        <v>8.4471304388306478</v>
       </c>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
@@ -3499,10 +3502,10 @@
       <c r="P8" s="13"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="43"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="13"/>
       <c r="J9" s="11"/>
       <c r="K9" s="14"/>
@@ -3520,21 +3523,21 @@
         <v>3.3</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="J10" s="42" t="s">
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="J10" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43" t="s">
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
       <c r="P10" s="13"/>
     </row>
     <row r="11" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3545,12 +3548,12 @@
         <v>7.2</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="F11" s="45" t="str">
+      <c r="F11" s="47" t="str">
         <f>Warnings!D4</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G11" s="46"/>
-      <c r="H11" s="47"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="49"/>
       <c r="J11" s="11"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
@@ -3563,9 +3566,9 @@
       <c r="B12" s="11"/>
       <c r="C12" s="14"/>
       <c r="D12" s="13"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
       <c r="J12" s="11"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
@@ -3575,14 +3578,14 @@
       <c r="P12" s="13"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="43"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="13"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="52"/>
       <c r="J13" s="11"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
@@ -3596,12 +3599,12 @@
         <v>45</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="52"/>
       <c r="J14" s="11"/>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
@@ -3618,9 +3621,9 @@
         <v>333</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="52"/>
       <c r="J15" s="11"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -3637,12 +3640,12 @@
         <v>25</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="F16" s="51" t="str">
+      <c r="F16" s="53" t="str">
         <f>IF(LEN(F11)&gt;1,"","No warnings.")</f>
         <v>No warnings.</v>
       </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="53"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="55"/>
       <c r="J16" s="11"/>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -3664,10 +3667,10 @@
       <c r="P17" s="13"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="43"/>
+      <c r="C18" s="39"/>
       <c r="D18" s="13"/>
       <c r="J18" s="11"/>
       <c r="K18" s="14"/>
@@ -3685,11 +3688,11 @@
         <v>0</v>
       </c>
       <c r="D19" s="13"/>
-      <c r="F19" s="44" t="s">
+      <c r="F19" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
       <c r="J19" s="11"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
@@ -3746,13 +3749,13 @@
         <v>5.7</v>
       </c>
       <c r="D22" s="13"/>
-      <c r="F22" s="54" t="s">
+      <c r="F22" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="G22" s="55" t="s">
+      <c r="G22" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="56"/>
+      <c r="H22" s="58"/>
       <c r="J22" s="11"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
@@ -3769,9 +3772,9 @@
         <v>10.8</v>
       </c>
       <c r="D23" s="13"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="58"/>
       <c r="J23" s="11"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -3862,7 +3865,7 @@
       </c>
       <c r="G27" s="38">
         <f>MAX(ChangeLog!A4:A1011)</f>
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="H27" s="21"/>
       <c r="J27" s="19"/>
@@ -3881,8 +3884,8 @@
         <v>9.1</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="11" t="s">
@@ -3911,13 +3914,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F4:H4"/>
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B9:C9"/>
@@ -3929,6 +3925,13 @@
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="G22:H23"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G22" r:id="rId1" xr:uid="{34DB199A-A3BF-4DC7-A0C6-1DB159FEB52F}"/>
@@ -4221,7 +4224,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4243,7 +4246,7 @@
         <v>Cattle</v>
       </c>
       <c r="C2" s="2">
-        <f>_xlfn.XMATCH(B2,Parameters!A3:A5)</f>
+        <f>MATCH(B2,Parameters!A3:A5,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -4253,11 +4256,11 @@
       </c>
       <c r="B3" t="str">
         <f>Model!C14</f>
-        <v>Tank</v>
+        <v>Lagoon</v>
       </c>
       <c r="C3" s="2">
-        <f>_xlfn.XMATCH(B3,Parameters!B2:C2)</f>
-        <v>2</v>
+        <f>MATCH(B3,Parameters!B2:C2,0)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4358,7 +4361,7 @@
       </c>
       <c r="F3" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G3" s="4">
         <f>Model!G$7</f>
@@ -4386,11 +4389,11 @@
       </c>
       <c r="M3" s="5">
         <f>1000*L3/F3*G3*86400</f>
-        <v>0.56663658004522821</v>
+        <v>0.62906264394851608</v>
       </c>
       <c r="N3" s="5">
         <f>M3*B3*H3/1000</f>
-        <v>5.8493894158068915</v>
+        <v>6.4938136734805321</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -4414,7 +4417,7 @@
       </c>
       <c r="F4" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G4" s="4">
         <f>Model!G$7</f>
@@ -4442,11 +4445,11 @@
       </c>
       <c r="M4" s="5">
         <f t="shared" ref="M4:M14" si="4">1000*L4/F4*G4*86400</f>
-        <v>0.56663658004522821</v>
+        <v>0.62906264394851608</v>
       </c>
       <c r="N4" s="5">
         <f t="shared" ref="N4:N14" si="5">M4*B4*H4/1000</f>
-        <v>5.3304919676304738</v>
+        <v>5.9177495572846777</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -4470,7 +4473,7 @@
       </c>
       <c r="F5" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G5" s="4">
         <f>Model!G$7</f>
@@ -4498,11 +4501,11 @@
       </c>
       <c r="M5" s="5">
         <f t="shared" si="4"/>
-        <v>0.75602636986463911</v>
+        <v>0.83931741061243825</v>
       </c>
       <c r="N5" s="5">
         <f t="shared" si="5"/>
-        <v>7.8044602161126697</v>
+        <v>8.6642736297522003</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -4526,7 +4529,7 @@
       </c>
       <c r="F6" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G6" s="4">
         <f>Model!G$7</f>
@@ -4554,11 +4557,11 @@
       </c>
       <c r="M6" s="5">
         <f t="shared" si="4"/>
-        <v>1.2258815416087741</v>
+        <v>1.3609362877182152</v>
       </c>
       <c r="N6" s="5">
         <f t="shared" si="5"/>
-        <v>12.246556600671653</v>
+        <v>13.59575351430497</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -4582,7 +4585,7 @@
       </c>
       <c r="F7" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G7" s="4">
         <f>Model!G$7</f>
@@ -4610,11 +4613,11 @@
       </c>
       <c r="M7" s="5">
         <f t="shared" si="4"/>
-        <v>2.3760609380508986</v>
+        <v>2.6378303634293871</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="5"/>
-        <v>24.528077063499428</v>
+        <v>27.230322841681563</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -4638,7 +4641,7 @@
       </c>
       <c r="F8" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G8" s="4">
         <f>Model!G$7</f>
@@ -4666,11 +4669,11 @@
       </c>
       <c r="M8" s="5">
         <f t="shared" si="4"/>
-        <v>3.6862972020553735</v>
+        <v>4.0924146904174066</v>
       </c>
       <c r="N8" s="5">
         <f t="shared" si="5"/>
-        <v>36.826109048533183</v>
+        <v>40.883222757269891</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -4694,7 +4697,7 @@
       </c>
       <c r="F9" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G9" s="4">
         <f>Model!G$7</f>
@@ -4722,11 +4725,11 @@
       </c>
       <c r="M9" s="5">
         <f t="shared" si="4"/>
-        <v>4.3263727569590307</v>
+        <v>4.8030070437426522</v>
       </c>
       <c r="N9" s="5">
         <f t="shared" si="5"/>
-        <v>44.661145970088079</v>
+        <v>49.581441712555403</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -4750,7 +4753,7 @@
       </c>
       <c r="F10" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G10" s="4">
         <f>Model!G$7</f>
@@ -4778,11 +4781,11 @@
       </c>
       <c r="M10" s="5">
         <f t="shared" si="4"/>
-        <v>4.3796932384542711</v>
+        <v>4.8622018155721145</v>
       </c>
       <c r="N10" s="5">
         <f t="shared" si="5"/>
-        <v>45.211573300563437</v>
+        <v>50.192509342150935</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -4806,7 +4809,7 @@
       </c>
       <c r="F11" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G11" s="4">
         <f>Model!G$7</f>
@@ -4834,11 +4837,11 @@
       </c>
       <c r="M11" s="5">
         <f t="shared" si="4"/>
-        <v>3.0202425172639424</v>
+        <v>3.3529810996743765</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="5"/>
-        <v>30.172222747466783</v>
+        <v>33.496281185747023</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -4862,7 +4865,7 @@
       </c>
       <c r="F12" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G12" s="4">
         <f>Model!G$7</f>
@@ -4890,11 +4893,11 @@
       </c>
       <c r="M12" s="5">
         <f t="shared" si="4"/>
-        <v>1.9112796878249705</v>
+        <v>2.1218443991955178</v>
       </c>
       <c r="N12" s="5">
         <f t="shared" si="5"/>
-        <v>19.730140217417169</v>
+        <v>21.90379973289533</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -4918,7 +4921,7 @@
       </c>
       <c r="F13" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G13" s="4">
         <f>Model!G$7</f>
@@ -4946,11 +4949,11 @@
       </c>
       <c r="M13" s="5">
         <f t="shared" si="4"/>
-        <v>1.0733346253077058</v>
+        <v>1.191583355214487</v>
       </c>
       <c r="N13" s="5">
         <f t="shared" si="5"/>
-        <v>10.722612906823983</v>
+        <v>11.903917718592725</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -4974,7 +4977,7 @@
       </c>
       <c r="F14" s="4">
         <f>Model!G$6</f>
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G14" s="4">
         <f>Model!G$7</f>
@@ -5002,11 +5005,11 @@
       </c>
       <c r="M14" s="5">
         <f t="shared" si="4"/>
-        <v>0.706168454826134</v>
+        <v>0.78396667442562329</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="5"/>
-        <v>7.2897769591701804</v>
+        <v>8.0928879800957088</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -5030,7 +5033,7 @@
       <c r="M15" s="5"/>
       <c r="N15" s="6">
         <f>SUM(N3:N14)</f>
-        <v>250.37255641378391</v>
+        <v>277.95597364581096</v>
       </c>
     </row>
   </sheetData>
@@ -5159,10 +5162,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252B4D1B-B8A9-457A-97D9-39EFD218058D}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5342,6 +5345,23 @@
         <v>114</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1.3</v>
+      </c>
+      <c r="B11" s="27">
+        <v>45156</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>